<commit_message>
add camera boom, camera and part of input functions
</commit_message>
<xml_diff>
--- a/GameDesign.xlsx
+++ b/GameDesign.xlsx
@@ -501,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -515,7 +515,7 @@
     <col min="4" max="4" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -523,7 +523,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -531,23 +534,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -555,25 +564,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
         <v>23</v>
@@ -582,28 +591,28 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
         <v>22</v>
@@ -612,14 +621,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" t="s">

</xml_diff>

<commit_message>
try to use enhanced input but not traditional way
</commit_message>
<xml_diff>
--- a/GameDesign.xlsx
+++ b/GameDesign.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>需要实现的功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,6 +170,10 @@
   </si>
   <si>
     <t>相机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用UE5的输入映射方式而不是UE4的</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -504,14 +508,14 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.375" customWidth="1"/>
     <col min="2" max="2" width="33.25" customWidth="1"/>
-    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="36.875" customWidth="1"/>
     <col min="4" max="4" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -549,6 +553,9 @@
       </c>
       <c r="B4" t="s">
         <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
I can look around and move around in the virual world !
</commit_message>
<xml_diff>
--- a/GameDesign.xlsx
+++ b/GameDesign.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA3A500-4989-438C-8F10-E7B52CF04735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>需要实现的功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -174,13 +175,24 @@
   </si>
   <si>
     <t>使用UE5的输入映射方式而不是UE4的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成基本的行走和四处看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
+  </si>
+  <si>
+    <t>已完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,11 +516,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -528,8 +540,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -539,8 +551,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>41</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
@@ -548,8 +560,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
migrate mesh, animations and some related things to this project, try to implement animation basic cpp next step
</commit_message>
<xml_diff>
--- a/GameDesign.xlsx
+++ b/GameDesign.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA3A500-4989-438C-8F10-E7B52CF04735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836BA117-79F0-4379-9423-065BF1B737CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>需要实现的功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,6 +186,22 @@
   </si>
   <si>
     <t>已完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动画蓝图类的cpp创建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已从第三人称模板中迁移动画</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在人物Cpp中实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在人物蓝图中实现</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -517,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -549,6 +565,9 @@
       <c r="C2" t="s">
         <v>36</v>
       </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -558,6 +577,9 @@
       <c r="C3" t="s">
         <v>37</v>
       </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -569,10 +591,19 @@
       <c r="C4" t="s">
         <v>38</v>
       </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -580,177 +611,183 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
+      <c r="C10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-      <c r="C19" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+      <c r="C21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
-      <c r="C22" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+      <c r="C24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
-      <c r="C28" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+      <c r="C29" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B6:B17"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="B6:B18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
I change the traditional logic about the state machine in the animation blueprint, try to use a signal but not the value to decide when and how to change the animation.Further more, I try to change the speed about the movement component based on the which animation is being played, I hope it will work
</commit_message>
<xml_diff>
--- a/GameDesign.xlsx
+++ b/GameDesign.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836BA117-79F0-4379-9423-065BF1B737CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCA402A-4922-4942-BA6D-B2B1B692273D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>需要实现的功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -202,6 +202,10 @@
   </si>
   <si>
     <t>在人物蓝图中实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动画的起步动作会有延时，即动画看起来起跑的速度是从0开始逐渐增加的，但是人物移动组件的速度却是一个恒定值。或许可以这样：移动组件的移动速度根据人物动画的移动步幅动态调整移动组件的移动速度。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -245,13 +249,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,21 +540,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.375" customWidth="1"/>
-    <col min="2" max="2" width="33.25" customWidth="1"/>
-    <col min="3" max="3" width="36.875" customWidth="1"/>
-    <col min="4" max="4" width="21.375" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -569,7 +577,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -581,7 +589,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -595,7 +603,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -606,7 +614,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -614,31 +622,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
         <v>23</v>
@@ -646,29 +654,35 @@
       <c r="D11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
         <v>22</v>
@@ -676,29 +690,33 @@
       <c r="D15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -706,19 +724,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
@@ -729,19 +747,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
@@ -749,7 +767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
         <v>12</v>
@@ -758,28 +776,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="E11:E18"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="B25:B29"/>

</xml_diff>